<commit_message>
we fucking finished bitchessssssssss
</commit_message>
<xml_diff>
--- a/contact.xlsx
+++ b/contact.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -34,31 +34,34 @@
     <t>id</t>
   </si>
   <si>
-    <t>tett</t>
+    <t>tt</t>
   </si>
   <si>
-    <t/>
+    <t>11</t>
   </si>
   <si>
-    <t>2022-03-17T09:14:59.586Z</t>
+    <t>2022-03-18T20:02:40.062Z</t>
   </si>
   <si>
-    <t>6231ef9a1aced32723d95284</t>
+    <t>6234e56efa1a37ad6b10fbb8</t>
   </si>
   <si>
-    <t>6232fc162479a3873cac1374</t>
+    <t>6234e57afa1a37ad6b10fbc1</t>
   </si>
   <si>
-    <t>2022-03-17T09:15:57.416Z</t>
+    <t>fawzi</t>
   </si>
   <si>
-    <t>6232fc51c0334fbf230d85ef</t>
+    <t>ttt</t>
   </si>
   <si>
-    <t>2022-03-17T09:17:56.644Z</t>
+    <t>1</t>
   </si>
   <si>
-    <t>6232fcc79350f23f5d3606ab</t>
+    <t>2022-03-18T20:27:31.009Z</t>
+  </si>
+  <si>
+    <t>6234eb4ed2906ab295e2fb29</t>
   </si>
 </sst>
 </file>
@@ -98,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showGridLines="1" workbookViewId="0" rightToLeft="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100"/>
   </sheetViews>
@@ -152,48 +155,25 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="0" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="F3" s="0" t="s">
         <v>10</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>